<commit_message>
Add petra V rotameter to worksheet
</commit_message>
<xml_diff>
--- a/etc/Booster_Interlock_EPICS_2.0.xlsx
+++ b/etc/Booster_Interlock_EPICS_2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23716"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25310"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranieri.santos\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnpemcamp.sharepoint.com/sites/rfq/Documentos Compartilhados/Variáveis EPICS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{056F9561-05DD-43E8-A554-60A9FC5F1B01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D544DFD0-006D-4FED-95D9-63C71B9E77E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-3300" windowWidth="29040" windowHeight="15990" xr2:uid="{0AE0F94C-E51D-461C-83D1-A0E4C349EF9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="4" activeTab="4" xr2:uid="{0AE0F94C-E51D-461C-83D1-A0E4C349EF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Interlock" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Petra 5" sheetId="4" r:id="rId5"/>
     <sheet name="Legenda" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,6 +32,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="254">
   <si>
     <t>Nº</t>
   </si>
@@ -107,48 +108,51 @@
     <t>Interlock Sirius</t>
   </si>
   <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>RaBO02</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>IntlkCtrl</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>IntlkSirius</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>.1</t>
+  </si>
+  <si>
+    <t>Sinal de erro do CLP para o LLRF</t>
+  </si>
+  <si>
+    <t>IntlkLLRF</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Sinal SSA Ligado para LLRF</t>
+  </si>
+  <si>
     <t>BO</t>
   </si>
   <si>
-    <t>RaBO02</t>
-  </si>
-  <si>
-    <t>RF</t>
-  </si>
-  <si>
-    <t>IntlkCtrl</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>IntlkSirius</t>
-  </si>
-  <si>
-    <t>Mon</t>
-  </si>
-  <si>
-    <t>Digital</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>.1</t>
-  </si>
-  <si>
-    <t>Sinal de erro do CLP para o LLRF</t>
-  </si>
-  <si>
-    <t>IntlkLLRF</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>Sinal SSA Ligado para LLRF</t>
-  </si>
-  <si>
     <t>05D</t>
   </si>
   <si>
@@ -179,9 +183,6 @@
     <t xml:space="preserve">Detector de Arco </t>
   </si>
   <si>
-    <t>RA</t>
-  </si>
-  <si>
     <t>TLBO</t>
   </si>
   <si>
@@ -518,15 +519,15 @@
     <t>LLRF</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Interlock CLP para o LLRF</t>
   </si>
   <si>
     <t>Termostato Pré-Amp 50 W</t>
   </si>
   <si>
+    <t>In</t>
+  </si>
+  <si>
     <t>PT - 100 01 Pré - Amplificador 50 W</t>
   </si>
   <si>
@@ -780,6 +781,12 @@
   </si>
   <si>
     <t>dBm</t>
+  </si>
+  <si>
+    <t>Rotametro Cavidade Petra V</t>
+  </si>
+  <si>
+    <t>Hd4FlwRt</t>
   </si>
   <si>
     <t>Variável que tenho dúvida</t>
@@ -1071,7 +1078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1242,6 +1249,37 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4412,8 +4450,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4FBF1CDA-7535-41E4-BB7C-C17937B9FAC2}" name="Table6" displayName="Table6" ref="A1:U37" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="A1:U37" xr:uid="{162E0020-C62D-46DF-87C0-62A7906D6373}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4FBF1CDA-7535-41E4-BB7C-C17937B9FAC2}" name="Table6" displayName="Table6" ref="A1:U38" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="A1:U38" xr:uid="{162E0020-C62D-46DF-87C0-62A7906D6373}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{06D6BAFE-CA0D-4B49-A034-A9F10C8C185B}" name="Nº" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{33E192F8-9B34-4961-B556-BF6CAFA3F3A2}" name="Description" dataDxfId="19"/>
@@ -4750,9 +4788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC3ED96-FC9E-46E9-9092-8505503A603D}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4761,8 +4797,9 @@
     <col min="10" max="10" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="30.42578125" customWidth="1"/>
     <col min="13" max="13" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="15.7109375" customWidth="1"/>
-    <col min="19" max="19" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4831,117 +4868,117 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="47" customFormat="1">
-      <c r="A2" s="34">
+    <row r="2" spans="1:21" s="70" customFormat="1">
+      <c r="A2" s="68">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="37" t="str">
+      <c r="J2" s="56" t="str">
         <f>IF(G2="-",C2&amp;"-"&amp;D2&amp;":"&amp;E2&amp;"-"&amp;F2&amp;":"&amp;H2&amp;"-"&amp;I2,C2&amp;"-"&amp;D2&amp;":"&amp;E2&amp;"-"&amp;F2&amp;"-"&amp;G2&amp;":"&amp;H2&amp;"-"&amp;I2)</f>
-        <v>BO-RaBO02:RF-IntlkCtrl:IntlkSirius-Mon</v>
-      </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38" t="str">
+        <v>RA-RaBO02:RF-IntlkCtrl:IntlkSirius-Mon</v>
+      </c>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57" t="str">
         <f>IF(G2="-",C2&amp;"_"&amp;D2&amp;"_"&amp;E2&amp;"_"&amp;F2&amp;"_"&amp;H2&amp;""&amp;I2,C2&amp;"_"&amp;D2&amp;"_"&amp;E2&amp;"_"&amp;F2&amp;"_"&amp;G2&amp;"_"&amp;H2&amp;""&amp;I2)</f>
-        <v>BO_RaBO02_RF_IntlkCtrl_IntlkSiriusMon</v>
-      </c>
-      <c r="N2" s="38" t="s">
+        <v>RA_RaBO02_RF_IntlkCtrl_IntlkSiriusMon</v>
+      </c>
+      <c r="N2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38" t="str">
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57" t="str">
         <f>M2</f>
-        <v>BO_RaBO02_RF_IntlkCtrl_IntlkSiriusMon</v>
-      </c>
-      <c r="T2" s="38" t="s">
+        <v>RA_RaBO02_RF_IntlkCtrl_IntlkSiriusMon</v>
+      </c>
+      <c r="T2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="39"/>
+      <c r="U2" s="69"/>
     </row>
-    <row r="3" spans="1:21" s="47" customFormat="1">
-      <c r="A3" s="48">
+    <row r="3" spans="1:21" s="70" customFormat="1">
+      <c r="A3" s="62">
         <v>2</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="51" t="str">
+      <c r="J3" s="65" t="str">
         <f>IF(G3="-",C3&amp;"-"&amp;D3&amp;":"&amp;E3&amp;"-"&amp;F3&amp;":"&amp;H3&amp;"-"&amp;I3,C3&amp;"-"&amp;D3&amp;":"&amp;E3&amp;"-"&amp;F3&amp;"-"&amp;G3&amp;":"&amp;H3&amp;"-"&amp;I3)</f>
-        <v>BO-RaBO02:RF-IntlkCtrl:IntlkLLRF-Mon</v>
-      </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52" t="str">
+        <v>RA-RaBO02:RF-IntlkCtrl:IntlkLLRF-Mon</v>
+      </c>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="66" t="str">
         <f>IF(G3="-",C3&amp;"_"&amp;D3&amp;"_"&amp;E3&amp;"_"&amp;F3&amp;"_"&amp;H3&amp;""&amp;I3,C3&amp;"_"&amp;D3&amp;"_"&amp;E3&amp;"_"&amp;F3&amp;"_"&amp;G3&amp;"_"&amp;H3&amp;""&amp;I3)</f>
-        <v>BO_RaBO02_RF_IntlkCtrl_IntlkLLRFMon</v>
-      </c>
-      <c r="N3" s="52" t="s">
+        <v>RA_RaBO02_RF_IntlkCtrl_IntlkLLRFMon</v>
+      </c>
+      <c r="N3" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="52" t="s">
+      <c r="O3" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52" t="str">
+      <c r="P3" s="66"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="66" t="str">
         <f t="shared" ref="S3:S6" si="0">M3</f>
-        <v>BO_RaBO02_RF_IntlkCtrl_IntlkLLRFMon</v>
-      </c>
-      <c r="T3" s="52" t="s">
+        <v>RA_RaBO02_RF_IntlkCtrl_IntlkLLRFMon</v>
+      </c>
+      <c r="T3" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="53"/>
+      <c r="U3" s="67"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="19">
@@ -4951,22 +4988,22 @@
         <v>35</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>28</v>
@@ -5004,25 +5041,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>26</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>28</v>
@@ -5055,61 +5092,61 @@
       </c>
       <c r="U5" s="20"/>
     </row>
-    <row r="6" spans="1:21" s="6" customFormat="1">
-      <c r="A6" s="48">
+    <row r="6" spans="1:21" s="58" customFormat="1">
+      <c r="A6" s="62">
         <v>5</v>
       </c>
-      <c r="B6" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="50" t="s">
+      <c r="B6" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="50" t="s">
+      <c r="F6" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="36" t="s">
+      <c r="H6" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="51" t="str">
+      <c r="I6" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="65" t="str">
         <f>IF(G6="-",C6&amp;"-"&amp;D6&amp;":"&amp;E6&amp;"-"&amp;F6&amp;":"&amp;H6&amp;"-"&amp;I6,C6&amp;"-"&amp;D6&amp;":"&amp;E6&amp;"-"&amp;F6&amp;"-"&amp;G6&amp;":"&amp;H6&amp;"-"&amp;I6)</f>
-        <v>BO-RaBO02:RF-Intlk:Reset-Cmd</v>
-      </c>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="52" t="str">
+        <v>RA-RaBO02:RF-Intlk:Reset-Cmd</v>
+      </c>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="66" t="str">
         <f>IF(G6="-",C6&amp;"_"&amp;D6&amp;"_"&amp;E6&amp;"_"&amp;F6&amp;"_"&amp;H6&amp;""&amp;I6,C6&amp;"_"&amp;D6&amp;"_"&amp;E6&amp;"_"&amp;F6&amp;"_"&amp;G6&amp;"_"&amp;H6&amp;""&amp;I6)</f>
-        <v>BO_RaBO02_RF_Intlk_ResetCmd</v>
-      </c>
-      <c r="N6" s="52" t="s">
+        <v>RA_RaBO02_RF_Intlk_ResetCmd</v>
+      </c>
+      <c r="N6" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52" t="str">
+      <c r="O6" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="66" t="str">
         <f t="shared" si="0"/>
-        <v>BO_RaBO02_RF_Intlk_ResetCmd</v>
-      </c>
-      <c r="T6" s="52" t="s">
+        <v>RA_RaBO02_RF_Intlk_ResetCmd</v>
+      </c>
+      <c r="T6" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="U6" s="53"/>
+      <c r="U6" s="67"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5125,9 +5162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CD3B42-ABB0-4480-B785-94CB22DEE6B9}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5219,10 +5254,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>47</v>
@@ -5278,7 +5313,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D3" s="31" t="s">
         <v>23</v>
@@ -5332,7 +5367,7 @@
         <v>55</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>23</v>
@@ -5353,20 +5388,20 @@
         <v>57</v>
       </c>
       <c r="J4" s="17" t="str">
-        <f t="shared" ref="J3:J16" si="1">IF(G4="-",C4&amp;"-"&amp;D4&amp;":"&amp;E4&amp;"-"&amp;F4&amp;":"&amp;H4&amp;"-"&amp;I4,C4&amp;"-"&amp;D4&amp;":"&amp;E4&amp;"-"&amp;F4&amp;"-"&amp;G4&amp;":"&amp;H4&amp;"-"&amp;I4)</f>
+        <f t="shared" ref="J4:J16" si="1">IF(G4="-",C4&amp;"-"&amp;D4&amp;":"&amp;E4&amp;"-"&amp;F4&amp;":"&amp;H4&amp;"-"&amp;I4,C4&amp;"-"&amp;D4&amp;":"&amp;E4&amp;"-"&amp;F4&amp;"-"&amp;G4&amp;":"&amp;H4&amp;"-"&amp;I4)</f>
         <v>RA-RaBO02:RF-ArcDetec-Circ:Test-Sel</v>
       </c>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="18" t="str">
-        <f t="shared" ref="M3:M16" si="2">IF(G4="-",C4&amp;"_"&amp;D4&amp;"_"&amp;E4&amp;"_"&amp;F4&amp;"_"&amp;H4&amp;""&amp;I4,C4&amp;"_"&amp;D4&amp;"_"&amp;E4&amp;"_"&amp;F4&amp;"_"&amp;G4&amp;"_"&amp;H4&amp;""&amp;I4)</f>
+        <f t="shared" ref="M4:M16" si="2">IF(G4="-",C4&amp;"_"&amp;D4&amp;"_"&amp;E4&amp;"_"&amp;F4&amp;"_"&amp;H4&amp;""&amp;I4,C4&amp;"_"&amp;D4&amp;"_"&amp;E4&amp;"_"&amp;F4&amp;"_"&amp;G4&amp;"_"&amp;H4&amp;""&amp;I4)</f>
         <v>RA_RaBO02_RF_ArcDetec_Circ_TestSel</v>
       </c>
       <c r="N4" s="18" t="s">
         <v>29</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
@@ -5388,7 +5423,7 @@
         <v>58</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>23</v>
@@ -5444,7 +5479,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>47</v>
@@ -5500,7 +5535,7 @@
         <v>62</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D7" s="36" t="s">
         <v>47</v>
@@ -5556,7 +5591,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>47</v>
@@ -5604,7 +5639,7 @@
       </c>
       <c r="U8" s="39"/>
     </row>
-    <row r="9" spans="1:21" s="6" customFormat="1">
+    <row r="9" spans="1:21" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="34">
         <v>8</v>
       </c>
@@ -5612,7 +5647,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>47</v>
@@ -5668,7 +5703,7 @@
         <v>67</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>47</v>
@@ -5724,7 +5759,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D11" s="36" t="s">
         <v>47</v>
@@ -5780,7 +5815,7 @@
         <v>71</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>47</v>
@@ -5836,7 +5871,7 @@
         <v>73</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>47</v>
@@ -5892,7 +5927,7 @@
         <v>75</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>47</v>
@@ -5946,7 +5981,7 @@
         <v>76</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>47</v>
@@ -5980,7 +6015,7 @@
         <v>29</v>
       </c>
       <c r="O15" s="38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
@@ -6002,7 +6037,7 @@
         <v>78</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>23</v>
@@ -6017,7 +6052,7 @@
         <v>52</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I16" s="16" t="s">
         <v>28</v>
@@ -6058,7 +6093,7 @@
         <v>79</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D17" s="50" t="s">
         <v>23</v>
@@ -6119,9 +6154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A36DD4F-5FD0-437C-8BA8-AE5315936B8D}">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6214,7 +6247,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>82</v>
@@ -6282,7 +6315,7 @@
         <v>85</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>82</v>
@@ -6315,14 +6348,14 @@
         <v>N/A</v>
       </c>
       <c r="M3" s="25" t="str">
-        <f t="shared" ref="M3:M16" si="3">IF(G3="-",C3&amp;"_"&amp;D3&amp;"_"&amp;E3&amp;"_"&amp;F3&amp;"_"&amp;H3&amp;""&amp;I3,C3&amp;"_"&amp;D3&amp;"_"&amp;E3&amp;"_"&amp;F3&amp;"_"&amp;G3&amp;"_"&amp;H3&amp;""&amp;I3)</f>
+        <f t="shared" ref="M3:M14" si="3">IF(G3="-",C3&amp;"_"&amp;D3&amp;"_"&amp;E3&amp;"_"&amp;F3&amp;"_"&amp;H3&amp;""&amp;I3,C3&amp;"_"&amp;D3&amp;"_"&amp;E3&amp;"_"&amp;F3&amp;"_"&amp;G3&amp;"_"&amp;H3&amp;""&amp;I3)</f>
         <v>RA_ToBO_RF_ACDCPanel_300VdcDsblSel</v>
       </c>
       <c r="N3" s="25" t="s">
         <v>29</v>
       </c>
       <c r="O3" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P3" s="25" t="s">
         <v>54</v>
@@ -6332,7 +6365,7 @@
       </c>
       <c r="R3" s="25"/>
       <c r="S3" s="25" t="str">
-        <f t="shared" ref="S3:S16" si="4">M3</f>
+        <f t="shared" ref="S3:S13" si="4">M3</f>
         <v>RA_ToBO_RF_ACDCPanel_300VdcDsblSel</v>
       </c>
       <c r="T3" s="25" t="s">
@@ -6350,7 +6383,7 @@
         <v>87</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>82</v>
@@ -6390,7 +6423,7 @@
         <v>29</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P4" s="18" t="s">
         <v>54</v>
@@ -6418,7 +6451,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>82</v>
@@ -6486,7 +6519,7 @@
         <v>90</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>82</v>
@@ -6554,7 +6587,7 @@
         <v>94</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>82</v>
@@ -6622,7 +6655,7 @@
         <v>96</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>82</v>
@@ -6690,7 +6723,7 @@
         <v>98</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>82</v>
@@ -6758,7 +6791,7 @@
         <v>100</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>82</v>
@@ -6826,7 +6859,7 @@
         <v>102</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D11" s="36" t="s">
         <v>82</v>
@@ -6894,7 +6927,7 @@
         <v>104</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>82</v>
@@ -6964,7 +6997,7 @@
         <v>110</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>82</v>
@@ -7034,7 +7067,7 @@
         <v>111</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D14" s="36" t="s">
         <v>82</v>
@@ -7104,7 +7137,7 @@
         <v>112</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>82</v>
@@ -7174,7 +7207,7 @@
         <v>113</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>82</v>
@@ -7244,7 +7277,7 @@
         <v>114</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D17" s="36" t="s">
         <v>82</v>
@@ -7314,7 +7347,7 @@
         <v>115</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>82</v>
@@ -7382,7 +7415,7 @@
         <v>117</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>82</v>
@@ -7450,7 +7483,7 @@
         <v>118</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>82</v>
@@ -7518,7 +7551,7 @@
         <v>119</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>82</v>
@@ -7586,7 +7619,7 @@
         <v>120</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>82</v>
@@ -7654,7 +7687,7 @@
         <v>121</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D23" s="16" t="s">
         <v>82</v>
@@ -7722,7 +7755,7 @@
         <v>122</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>82</v>
@@ -7790,7 +7823,7 @@
         <v>124</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D25" s="16" t="s">
         <v>82</v>
@@ -7858,7 +7891,7 @@
         <v>125</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>82</v>
@@ -7926,7 +7959,7 @@
         <v>126</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>82</v>
@@ -7994,7 +8027,7 @@
         <v>127</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>82</v>
@@ -8062,7 +8095,7 @@
         <v>128</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>82</v>
@@ -8130,7 +8163,7 @@
         <v>129</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>82</v>
@@ -8198,7 +8231,7 @@
         <v>132</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>82</v>
@@ -8238,7 +8271,7 @@
         <v>29</v>
       </c>
       <c r="O31" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P31" s="18" t="s">
         <v>54</v>
@@ -8266,7 +8299,7 @@
         <v>134</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>82</v>
@@ -8306,7 +8339,7 @@
         <v>29</v>
       </c>
       <c r="O32" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P32" s="18" t="s">
         <v>54</v>
@@ -8334,7 +8367,7 @@
         <v>136</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>82</v>
@@ -8402,7 +8435,7 @@
         <v>138</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>82</v>
@@ -8442,7 +8475,7 @@
         <v>29</v>
       </c>
       <c r="O34" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P34" s="18" t="s">
         <v>54</v>
@@ -8470,7 +8503,7 @@
         <v>139</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>82</v>
@@ -8540,7 +8573,7 @@
         <v>143</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>82</v>
@@ -8610,7 +8643,7 @@
         <v>145</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D37" s="36" t="s">
         <v>82</v>
@@ -8678,7 +8711,7 @@
         <v>147</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D38" s="50" t="s">
         <v>82</v>
@@ -8693,7 +8726,7 @@
         <v>26</v>
       </c>
       <c r="H38" s="50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I38" s="50" t="s">
         <v>28</v>
@@ -8751,16 +8784,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC95139-34C0-46F8-976D-0942B4E97D5D}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="42.7109375" customWidth="1"/>
     <col min="13" max="13" width="41.42578125" bestFit="1" customWidth="1"/>
@@ -8844,7 +8881,7 @@
         <v>148</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D2" s="55" t="s">
         <v>149</v>
@@ -8862,7 +8899,7 @@
         <v>151</v>
       </c>
       <c r="I2" s="55" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J2" s="56" t="str">
         <f>IF(G2="-",C2&amp;"-"&amp;D2&amp;":"&amp;E2&amp;"-"&amp;F2&amp;":"&amp;H2&amp;"-"&amp;I2,C2&amp;"-"&amp;D2&amp;":"&amp;E2&amp;"-"&amp;F2&amp;"-"&amp;G2&amp;":"&amp;H2&amp;"-"&amp;I2)</f>
@@ -8884,7 +8921,7 @@
         <v>29</v>
       </c>
       <c r="O2" s="57" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P2" s="57"/>
       <c r="Q2" s="57"/>
@@ -8906,7 +8943,7 @@
         <v>152</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D3" s="55" t="s">
         <v>149</v>
@@ -8924,7 +8961,7 @@
         <v>153</v>
       </c>
       <c r="I3" s="55" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J3" s="56" t="str">
         <f t="shared" ref="J3:J12" si="2">IF(G3="-",C3&amp;"-"&amp;D3&amp;":"&amp;E3&amp;"-"&amp;F3&amp;":"&amp;H3&amp;"-"&amp;I3,C3&amp;"-"&amp;D3&amp;":"&amp;E3&amp;"-"&amp;F3&amp;"-"&amp;G3&amp;":"&amp;H3&amp;"-"&amp;I3)</f>
@@ -8946,7 +8983,7 @@
         <v>29</v>
       </c>
       <c r="O3" s="57" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P3" s="57"/>
       <c r="Q3" s="57"/>
@@ -8968,7 +9005,7 @@
         <v>154</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>149</v>
@@ -9025,7 +9062,7 @@
         <v>156</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>149</v>
@@ -9079,138 +9116,138 @@
       </c>
       <c r="U5" s="18"/>
     </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="14">
+    <row r="6" spans="1:21" s="58" customFormat="1">
+      <c r="A6" s="59">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>RA-RaBO01:RF-LLRF:Intlk-Mon</v>
+      </c>
+      <c r="K6" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="L6" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="M6" s="57" t="str">
+        <f t="shared" si="3"/>
+        <v>RA_RaBO01_RF_LLRF_IntlkMon</v>
+      </c>
+      <c r="N6" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57" t="str">
+        <f>M6</f>
+        <v>RA_RaBO01_RF_LLRF_IntlkMon</v>
+      </c>
+      <c r="T6" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" s="57"/>
+    </row>
+    <row r="7" spans="1:21" s="61" customFormat="1">
+      <c r="A7" s="60">
+        <v>6</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="D7" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F7" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G7" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="I6" s="16" t="s">
+      <c r="H7" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>BO-05D:RF-LLRF:Status-Mon</v>
-      </c>
-      <c r="K6" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>N/A</v>
-      </c>
-      <c r="L6" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
-      <c r="M6" s="18" t="str">
-        <f t="shared" si="3"/>
-        <v>BO_05D_RF_LLRF_StatusMon</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18" t="str">
-        <f>M6</f>
-        <v>BO_05D_RF_LLRF_StatusMon</v>
-      </c>
-      <c r="T6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="U6" s="18"/>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="14">
-        <v>6</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="17" t="str">
+      <c r="J7" s="60" t="str">
         <f t="shared" si="2"/>
         <v>BO-05D:RF-LLRF:Intlk-Mon</v>
       </c>
-      <c r="K7" s="17" t="str">
+      <c r="K7" s="60" t="str">
         <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
-      <c r="L7" s="17" t="str">
+      <c r="L7" s="60" t="str">
         <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
-      <c r="M7" s="18" t="str">
+      <c r="M7" s="60" t="str">
         <f t="shared" si="3"/>
         <v>BO_05D_RF_LLRF_IntlkMon</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="T7" s="18" t="s">
+      <c r="P7" s="60"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="T7" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="U7" s="18"/>
+      <c r="U7" s="60"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>149</v>
@@ -9242,9 +9279,8 @@
         <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
-      <c r="M8" s="18" t="str">
-        <f t="shared" si="3"/>
-        <v>RA_RaBO01_RF_LLRFPreAmp_TmsMon</v>
+      <c r="M8" s="18" t="s">
+        <v>161</v>
       </c>
       <c r="N8" s="18" t="s">
         <v>29</v>
@@ -9271,7 +9307,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>149</v>
@@ -9339,7 +9375,7 @@
         <v>165</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>149</v>
@@ -9396,7 +9432,7 @@
         <v>167</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>149</v>
@@ -9457,7 +9493,7 @@
         <v>169</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>149</v>
@@ -9522,10 +9558,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF9A12A-5087-484F-9B5F-D3D6B631F998}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="L26" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9616,10 +9652,10 @@
         <v>171</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>24</v>
@@ -9645,7 +9681,7 @@
         <v>N/A</v>
       </c>
       <c r="L2" s="17" t="str">
-        <f t="shared" ref="L2:L38" si="0">IF(OR(Q2="",Q2="N/A"),"N/A",IF(G2="-",C2&amp;"-"&amp;D2&amp;":"&amp;E2&amp;"-"&amp;F2&amp;":"&amp;H2&amp;"LowerLimit-Cte",C2&amp;"-"&amp;D2&amp;":"&amp;E2&amp;"-"&amp;F2&amp;"-"&amp;G2&amp;":"&amp;H2&amp;"LowerLimit-Cte"))</f>
+        <f t="shared" ref="L2:L37" si="0">IF(OR(Q2="",Q2="N/A"),"N/A",IF(G2="-",C2&amp;"-"&amp;D2&amp;":"&amp;E2&amp;"-"&amp;F2&amp;":"&amp;H2&amp;"LowerLimit-Cte",C2&amp;"-"&amp;D2&amp;":"&amp;E2&amp;"-"&amp;F2&amp;"-"&amp;G2&amp;":"&amp;H2&amp;"LowerLimit-Cte"))</f>
         <v>N/A</v>
       </c>
       <c r="M2" s="18" t="str">
@@ -9656,7 +9692,7 @@
         <v>29</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>54</v>
@@ -9682,10 +9718,10 @@
         <v>173</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>24</v>
@@ -9707,7 +9743,7 @@
         <v>BO-05D:RF-P5Cav:Hd1FlwRt-Mon</v>
       </c>
       <c r="K3" s="24" t="str">
-        <f t="shared" ref="K3:K38" si="2">IF(OR(P3="",P3="N/A"),"N/A",IF(G3="-",C3&amp;"-"&amp;D3&amp;":"&amp;E3&amp;"-"&amp;F3&amp;":"&amp;H3&amp;"UpperLimit-Cte",C3&amp;"-"&amp;D3&amp;":"&amp;E3&amp;"-"&amp;F3&amp;"-"&amp;G3&amp;":"&amp;H3&amp;"UpperLimit-Cte"))</f>
+        <f t="shared" ref="K3:K37" si="2">IF(OR(P3="",P3="N/A"),"N/A",IF(G3="-",C3&amp;"-"&amp;D3&amp;":"&amp;E3&amp;"-"&amp;F3&amp;":"&amp;H3&amp;"UpperLimit-Cte",C3&amp;"-"&amp;D3&amp;":"&amp;E3&amp;"-"&amp;F3&amp;"-"&amp;G3&amp;":"&amp;H3&amp;"UpperLimit-Cte"))</f>
         <v>N/A</v>
       </c>
       <c r="L3" s="24" t="str">
@@ -9748,10 +9784,10 @@
         <v>175</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>24</v>
@@ -9814,10 +9850,10 @@
         <v>177</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>24</v>
@@ -9880,10 +9916,10 @@
         <v>179</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>24</v>
@@ -9950,10 +9986,10 @@
         <v>183</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>24</v>
@@ -10016,10 +10052,10 @@
         <v>185</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>24</v>
@@ -10082,10 +10118,10 @@
         <v>187</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>24</v>
@@ -10152,10 +10188,10 @@
         <v>190</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>24</v>
@@ -10222,10 +10258,10 @@
         <v>192</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>24</v>
@@ -10292,10 +10328,10 @@
         <v>194</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>24</v>
@@ -10362,10 +10398,10 @@
         <v>196</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>24</v>
@@ -10432,10 +10468,10 @@
         <v>198</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>24</v>
@@ -10498,10 +10534,10 @@
         <v>200</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>24</v>
@@ -10564,10 +10600,10 @@
         <v>202</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>24</v>
@@ -10630,10 +10666,10 @@
         <v>204</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>24</v>
@@ -10696,10 +10732,10 @@
         <v>206</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>24</v>
@@ -10762,10 +10798,10 @@
         <v>208</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>24</v>
@@ -10828,10 +10864,10 @@
         <v>210</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>24</v>
@@ -10894,10 +10930,10 @@
         <v>212</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>24</v>
@@ -10960,10 +10996,10 @@
         <v>214</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="16" t="s">
         <v>24</v>
@@ -11026,10 +11062,10 @@
         <v>216</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="16" t="s">
         <v>24</v>
@@ -11092,10 +11128,10 @@
         <v>218</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="16" t="s">
         <v>24</v>
@@ -11158,10 +11194,10 @@
         <v>220</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>24</v>
@@ -11224,10 +11260,10 @@
         <v>222</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>24</v>
@@ -11290,10 +11326,10 @@
         <v>224</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>24</v>
@@ -11356,10 +11392,10 @@
         <v>226</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>24</v>
@@ -11422,10 +11458,10 @@
         <v>228</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>24</v>
@@ -11488,10 +11524,10 @@
         <v>230</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>24</v>
@@ -11554,10 +11590,10 @@
         <v>232</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>24</v>
@@ -11620,10 +11656,10 @@
         <v>234</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>24</v>
@@ -11686,10 +11722,10 @@
         <v>236</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>24</v>
@@ -11752,10 +11788,10 @@
         <v>238</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E34" s="16" t="s">
         <v>24</v>
@@ -11818,10 +11854,10 @@
         <v>240</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>24</v>
@@ -11884,10 +11920,10 @@
         <v>242</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>24</v>
@@ -11950,10 +11986,10 @@
         <v>244</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>24</v>
@@ -12011,6 +12047,72 @@
       <c r="U37" s="25">
         <v>4</v>
       </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" s="46">
+        <v>37</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="24" t="str">
+        <f>IF(G38="-",C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;":"&amp;H38&amp;"-"&amp;I38,C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;"-"&amp;G38&amp;":"&amp;H38&amp;"-"&amp;I38)</f>
+        <v>BO-05D:RF-P5Cav:Hd4FlwRt-Mon</v>
+      </c>
+      <c r="K38" s="24" t="str">
+        <f>IF(OR(P38="",P38="N/A"),"N/A",IF(G38="-",C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;":"&amp;H38&amp;"UpperLimit-Cte",C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;"-"&amp;G38&amp;":"&amp;H38&amp;"UpperLimit-Cte"))</f>
+        <v>N/A</v>
+      </c>
+      <c r="L38" s="24" t="str">
+        <f>IF(OR(Q38="",Q38="N/A"),"N/A",IF(G38="-",C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;":"&amp;H38&amp;"LowerLimit-Cte",C38&amp;"-"&amp;D38&amp;":"&amp;E38&amp;"-"&amp;F38&amp;"-"&amp;G38&amp;":"&amp;H38&amp;"LowerLimit-Cte"))</f>
+        <v>N/A</v>
+      </c>
+      <c r="M38" s="25" t="str">
+        <f>IF(G38="-",C38&amp;"_"&amp;D38&amp;"_"&amp;E38&amp;"_"&amp;F38&amp;"_"&amp;H38&amp;""&amp;I38,C38&amp;"_"&amp;D38&amp;"_"&amp;E38&amp;"_"&amp;F38&amp;"_"&amp;G38&amp;"_"&amp;H38&amp;""&amp;I38)</f>
+        <v>BO_05D_RF_P5Cav_Hd4FlwRtMon</v>
+      </c>
+      <c r="N38" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="O38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q38" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="R38" s="25"/>
+      <c r="S38" s="25" t="str">
+        <f>M38</f>
+        <v>BO_05D_RF_P5Cav_Hd4FlwRtMon</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="U38" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -12036,27 +12138,27 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="30">
       <c r="B3" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="30">
       <c r="B4" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -12065,17 +12167,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001FADEDC2238D1B459B3876E2C2E99497" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="013df61940af3924e726a3aaea789461">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40443515-7982-453e-8cc3-61a478897d4d" xmlns:ns3="32dc2326-b69f-4ff3-bc41-ce299fdac243" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3892681982c38a39a14241091d0c9fbe" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001FADEDC2238D1B459B3876E2C2E99497" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="185fbcca694157d48c5e2d9efddd7c80">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40443515-7982-453e-8cc3-61a478897d4d" xmlns:ns3="32dc2326-b69f-4ff3-bc41-ce299fdac243" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="de311a658b2d625d2db377de3cccb77f" ns2:_="" ns3:_="">
     <xsd:import namespace="40443515-7982-453e-8cc3-61a478897d4d"/>
     <xsd:import namespace="32dc2326-b69f-4ff3-bc41-ce299fdac243"/>
     <xsd:element name="properties">
@@ -12096,6 +12189,7 @@
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -12106,7 +12200,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="40443515-7982-453e-8cc3-61a478897d4d" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Compartilhado com" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Compartilhado com" ma:description="" ma:hidden="true" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -12125,11 +12219,9 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:description="" ma:hidden="true" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -12151,19 +12243,17 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:hidden="true" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="MediaServiceOCR" ma:hidden="true" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+    <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:hidden="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -12183,11 +12273,14 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:hidden="true" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -12200,8 +12293,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -12290,7 +12383,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="40443515-7982-453e-8cc3-61a478897d4d">
@@ -12304,14 +12397,23 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{813B4F1D-6C0A-4BF0-A4A1-DF8E596259AD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C127A3B2-E076-4D2E-9077-D443D31C23C8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CDBADB4-A5DD-4D9C-8EAB-8DB5A61E5B22}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A178A6D-B2A5-4562-B3CC-AAC941779779}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A178A6D-B2A5-4562-B3CC-AAC941779779}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{813B4F1D-6C0A-4BF0-A4A1-DF8E596259AD}"/>
 </file>
</xml_diff>